<commit_message>
Update edited session - 2025-08-14T07:19:04.192Z - Cache Bust: 1755155944192
</commit_message>
<xml_diff>
--- a/log_history/Y1_B2223_Anatomy_checklist1755155899359_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
+++ b/log_history/Y1_B2223_Anatomy_checklist1755155899359_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,7 +424,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>232002</v>
+        <v>232003</v>
       </c>
       <c r="B2" t="str">
         <v>Anatomy</v>
@@ -436,15 +436,15 @@
         <v>10:18:24</v>
       </c>
       <c r="E2" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F2" t="str">
-        <v>admin@admin.com</v>
+        <v>5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>232003</v>
+        <v>232004</v>
       </c>
       <c r="B3" t="str">
         <v>Anatomy</v>
@@ -456,15 +456,15 @@
         <v>10:18:24</v>
       </c>
       <c r="E3" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F3" t="str">
-        <v>admin@admin.com</v>
+        <v>5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>232004</v>
+        <v>232005</v>
       </c>
       <c r="B4" t="str">
         <v>Anatomy</v>
@@ -473,38 +473,18 @@
         <v>14/08/2025</v>
       </c>
       <c r="D4" t="str">
-        <v>10:18:24</v>
+        <v>10:18:25</v>
       </c>
       <c r="E4" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F4" t="str">
-        <v>admin@admin.com</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>232005</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C5" t="str">
-        <v>14/08/2025</v>
-      </c>
-      <c r="D5" t="str">
-        <v>10:18:25</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Selection</v>
-      </c>
-      <c r="F5" t="str">
-        <v>admin@admin.com</v>
+        <v>5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-08-14T07:21:50.141Z - Cache Bust: 1755156110141
</commit_message>
<xml_diff>
--- a/log_history/Y1_B2223_Anatomy_checklist1755155899359_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
+++ b/log_history/Y1_B2223_Anatomy_checklist1755155899359_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -439,12 +439,12 @@
         <v>Scan</v>
       </c>
       <c r="F2" t="str">
-        <v>5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326</v>
+        <v>admin@admin.com</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>232004</v>
+        <v>232005</v>
       </c>
       <c r="B3" t="str">
         <v>Anatomy</v>
@@ -453,38 +453,18 @@
         <v>14/08/2025</v>
       </c>
       <c r="D3" t="str">
-        <v>10:18:24</v>
+        <v>10:18:25</v>
       </c>
       <c r="E3" t="str">
         <v>Scan</v>
       </c>
       <c r="F3" t="str">
-        <v>5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>232005</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C4" t="str">
-        <v>14/08/2025</v>
-      </c>
-      <c r="D4" t="str">
-        <v>10:18:25</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F4" t="str">
-        <v>5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326</v>
+        <v>admin@admin.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-08-14T07:29:43.655Z - Cache Bust ID: 1755156583655fcwn5s8ry
</commit_message>
<xml_diff>
--- a/log_history/Y1_B2223_Anatomy_checklist1755155899359_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
+++ b/log_history/Y1_B2223_Anatomy_checklist1755155899359_5edfa2692bdacc5e6ee805c626c50cb44cebb065f092d9a1067d89f74dacd326.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,7 +424,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>232003</v>
+        <v>232005</v>
       </c>
       <c r="B2" t="str">
         <v>Anatomy</v>
@@ -433,38 +433,18 @@
         <v>14/08/2025</v>
       </c>
       <c r="D2" t="str">
-        <v>10:18:24</v>
+        <v>10:18:25</v>
       </c>
       <c r="E2" t="str">
         <v>Scan</v>
       </c>
       <c r="F2" t="str">
-        <v>admin@admin.com</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>232005</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Anatomy</v>
-      </c>
-      <c r="C3" t="str">
-        <v>14/08/2025</v>
-      </c>
-      <c r="D3" t="str">
-        <v>10:18:25</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F3" t="str">
         <v>admin@admin.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>